<commit_message>
POM updated Excel file updated
</commit_message>
<xml_diff>
--- a/src/test/java/pages/Pages.xlsx
+++ b/src/test/java/pages/Pages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
   <si>
     <t>ElementName</t>
   </si>
@@ -349,6 +349,21 @@
   </si>
   <si>
     <t>9069345300</t>
+  </si>
+  <si>
+    <t>7730002117</t>
+  </si>
+  <si>
+    <t>5392726521</t>
+  </si>
+  <si>
+    <t>6076706315</t>
+  </si>
+  <si>
+    <t>8481652086</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1033</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1208,7 @@
         <v>42</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1221,7 +1236,7 @@
         <v>44</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1279,7 +1294,7 @@
         <v>52</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
POM and Excel file updated
</commit_message>
<xml_diff>
--- a/src/test/java/pages/Pages.xlsx
+++ b/src/test/java/pages/Pages.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poorn\OneDrive\Desktop\AVIV\Aviv-QA-Web-Technical-Test\src\test\java\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3BEEA92-5F9A-4182-B8B8-E87AAEF36164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B7521A2-44A3-4799-86B2-56A7F3B6B52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVIV_Registration" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="93">
   <si>
     <t>ElementName</t>
   </si>
@@ -201,9 +201,6 @@
     <t>123143</t>
   </si>
   <si>
-    <t>2342</t>
-  </si>
-  <si>
     <t>//*[@id="shipping-method-buttons-container"]/button</t>
   </si>
   <si>
@@ -309,68 +306,13 @@
     <t>//img[@src='https://demo.nopcommerce.com/images/thumbs/0000053_adidas-consortium-campus-80s-running-shoes_80.jpg']//following::a[text()='Edit']</t>
   </si>
   <si>
-    <t>7268391293</t>
-  </si>
-  <si>
-    <t>9108077070</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER: 1035</t>
-  </si>
-  <si>
-    <t>5817218439</t>
-  </si>
-  <si>
-    <t>8038298082</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER: 1031</t>
-  </si>
-  <si>
-    <t>9568637702</t>
-  </si>
-  <si>
-    <t>4246207533</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER: 1032</t>
-  </si>
-  <si>
-    <t>1222194733</t>
-  </si>
-  <si>
-    <t>9577158214</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER: 1034</t>
-  </si>
-  <si>
-    <t>2136580454</t>
-  </si>
-  <si>
-    <t>9069345300</t>
-  </si>
-  <si>
-    <t>7730002117</t>
-  </si>
-  <si>
-    <t>5392726521</t>
-  </si>
-  <si>
-    <t>6076706315</t>
-  </si>
-  <si>
-    <t>8481652086</t>
-  </si>
-  <si>
-    <t>ORDER NUMBER: 1033</t>
+    <t>675</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -702,62 +644,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.21875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>65</v>
-      </c>
-    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -765,75 +707,75 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
+      <c r="A10" t="s">
         <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -855,34 +797,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5546875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.77734375"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -890,38 +832,38 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -937,51 +879,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD31F36-5E01-4999-A934-E0C69F9FDF65}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="50.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -989,127 +931,127 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="0">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="D9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>78</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>77</v>
-      </c>
-      <c r="D9" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>80</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>91</v>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1121,62 +1063,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB218D8-12AC-4D42-8E46-A8A1EB3EC80B}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.109375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="62.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="130.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1184,41 +1126,41 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s" s="0">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s" s="0">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>109</v>
+      <c r="D6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s" s="0">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1226,130 +1168,130 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s" s="0">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s" s="0">
-        <v>110</v>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="0">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="0">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>61</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="0">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>67</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="0">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>88</v>
       </c>
-      <c r="B17" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>92</v>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated step Definition files with new step definitions
</commit_message>
<xml_diff>
--- a/src/test/java/pages/Pages.xlsx
+++ b/src/test/java/pages/Pages.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poorn\OneDrive\Desktop\AVIV\Aviv-QA-Web-Technical-Test\src\test\java\pages\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t>ElementName</t>
   </si>
@@ -307,12 +307,67 @@
   </si>
   <si>
     <t>675</t>
+  </si>
+  <si>
+    <t>4811811531</t>
+  </si>
+  <si>
+    <t>3703609620</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1032</t>
+  </si>
+  <si>
+    <t>8159175216</t>
+  </si>
+  <si>
+    <t>3119770060</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1033</t>
+  </si>
+  <si>
+    <t>3973249268</t>
+  </si>
+  <si>
+    <t>4438734480</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1034</t>
+  </si>
+  <si>
+    <t>5537260889</t>
+  </si>
+  <si>
+    <t>1933791717</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1035</t>
+  </si>
+  <si>
+    <t>4725967011</t>
+  </si>
+  <si>
+    <t>9055273195</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1037</t>
+  </si>
+  <si>
+    <t>3109847671</t>
+  </si>
+  <si>
+    <t>5064293205</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1038</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -644,62 +699,62 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.21875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -707,13 +762,13 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -721,13 +776,13 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -735,46 +790,46 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>68</v>
       </c>
     </row>
@@ -797,34 +852,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -832,13 +887,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -846,24 +901,24 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>45</v>
       </c>
     </row>
@@ -885,45 +940,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="50.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -931,126 +986,126 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="0">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="0">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="0">
         <v>90</v>
       </c>
     </row>
@@ -1069,56 +1124,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="130.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.21875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="130.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1126,41 +1181,41 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
-        <v>67</v>
+      <c r="D6" t="s" s="0">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s" s="0">
         <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1168,129 +1223,129 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
+      <c r="D8" t="s" s="0">
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="0">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>92</v>
+      <c r="D13" t="s" s="0">
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="0">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="0">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s" s="0">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s" s="0">
         <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>88</v>
       </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s" s="0">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Take screenshot for all steps
</commit_message>
<xml_diff>
--- a/src/test/java/pages/Pages.xlsx
+++ b/src/test/java/pages/Pages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
   <si>
     <t>ElementName</t>
   </si>
@@ -361,6 +361,21 @@
   </si>
   <si>
     <t>ORDER NUMBER: 1038</t>
+  </si>
+  <si>
+    <t>6776279900</t>
+  </si>
+  <si>
+    <t>4555277731</t>
+  </si>
+  <si>
+    <t>ORDER NUMBER: 1036</t>
+  </si>
+  <si>
+    <t>5524032318</t>
+  </si>
+  <si>
+    <t>4199964175</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1220,7 @@
         <v>42</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1233,7 +1248,7 @@
         <v>44</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,7 +1306,7 @@
         <v>52</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Base Test and Utilities added
</commit_message>
<xml_diff>
--- a/src/test/java/pages/Pages.xlsx
+++ b/src/test/java/pages/Pages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
   <si>
     <t>ElementName</t>
   </si>
@@ -376,6 +376,18 @@
   </si>
   <si>
     <t>4199964175</t>
+  </si>
+  <si>
+    <t>9481895350</t>
+  </si>
+  <si>
+    <t>4196513918</t>
+  </si>
+  <si>
+    <t>3518152942</t>
+  </si>
+  <si>
+    <t>5894143326</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1232,7 @@
         <v>42</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1248,7 +1260,7 @@
         <v>44</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1306,7 +1318,7 @@
         <v>52</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>